<commit_message>
html log added and changed made in code for the same
</commit_message>
<xml_diff>
--- a/src/main/resources/AmazePOSData.xlsx
+++ b/src/main/resources/AmazePOSData.xlsx
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="BO User" sheetId="2" r:id="rId2"/>
+    <sheet name="InvalidCharacters" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
@@ -43,12 +43,180 @@
   <si>
     <t>amazeqa</t>
   </si>
+  <si>
+    <t>First Name</t>
+  </si>
+  <si>
+    <t>Middle Name</t>
+  </si>
+  <si>
+    <t>Last Name</t>
+  </si>
+  <si>
+    <t>Display Name</t>
+  </si>
+  <si>
+    <t>Employee ID</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Country Code</t>
+  </si>
+  <si>
+    <t>Phone Number</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Extension</t>
+  </si>
+  <si>
+    <t>Change Password</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Departmen</t>
+  </si>
+  <si>
+    <t>Designation</t>
+  </si>
+  <si>
+    <t>Invalid Data</t>
+  </si>
+  <si>
+    <t>~`!</t>
+  </si>
+  <si>
+    <t>~!@</t>
+  </si>
+  <si>
+    <t>Field Name</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>@</t>
+  </si>
+  <si>
+    <t>#</t>
+  </si>
+  <si>
+    <t>~`!@#$%^&amp;*()_+=-[{]}]]\|;:'"/?.&gt;,&lt;</t>
+  </si>
+  <si>
+    <t>$</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>=</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>[</t>
+  </si>
+  <si>
+    <t>{</t>
+  </si>
+  <si>
+    <t>]</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>\</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>;</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>/</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>.</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>,</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">     </t>
+  </si>
+  <si>
+    <t>Special Characters</t>
+  </si>
+  <si>
+    <t>Numbers</t>
+  </si>
+  <si>
+    <t>Decimal</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -56,16 +224,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <color rgb="FFFF0000"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -73,12 +263,119 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
+    <border diagonalDown="false" diagonalUp="false">
+      <left style="thin"/>
+      <right style="none"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal style="none"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom" horizontal="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="bottom" horizontal="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="bottom" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="center" horizontal="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="center" horizontal="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="0" applyFill="1" borderId="1" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="3" applyBorder="1" applyAlignment="1" applyProtection="1" xfId="0">
+      <alignment vertical="center"/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" fillId="2" applyFill="1" borderId="2" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0" quotePrefix="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="0" applyFill="1" borderId="0" applyBorder="1" applyAlignment="1" xfId="0" quotePrefix="1">
+      <alignment vertical="center" horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -395,7 +692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
@@ -430,10 +727,115 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1">
+      <selection activeCell="B2" sqref="B2" activeCellId="0"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.332" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" width="9.88672" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" width="12" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" width="9.44141" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" width="12.1094" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" width="11.2188" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" width="5.44141" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" width="12.1094" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" width="6.10938" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" width="10" customWidth="1" bestFit="1"/>
+    <col min="14" max="14" width="15.332" customWidth="1" bestFit="1"/>
+    <col min="16" max="16" width="11.4414" customWidth="1" bestFit="1"/>
+    <col min="17" max="17" width="4.55469" customWidth="1" bestFit="1"/>
+    <col min="18" max="18" width="10.332" customWidth="1" bestFit="1"/>
+    <col min="19" max="19" width="10.5547" customWidth="1" bestFit="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -442,10 +844,232 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A1" tabSelected="1">
+      <selection activeCell="A2" activeCellId="0" sqref="A2:A35"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="15.8867" customWidth="1" bestFit="1" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="1" s="15">
+      <c r="A1" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" customFormat="1" s="15">
+      <c r="A2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="15">
+        <v>0</v>
+      </c>
+      <c r="C2" s="15">
+        <v>1E-2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="1" s="15">
+      <c r="A3" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="1" s="15">
+      <c r="A4" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" customFormat="1" s="15">
+      <c r="A5" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="1" s="15">
+      <c r="A6" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" customFormat="1" s="15">
+      <c r="A7" s="15" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" customFormat="1" s="15">
+      <c r="A8" s="15" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="15">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" customFormat="1" s="15">
+      <c r="A9" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="1" s="15">
+      <c r="A10" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" customFormat="1" s="15">
+      <c r="A11" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="15">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" s="15">
+      <c r="A12" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" s="15">
+      <c r="A13" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" customFormat="1" s="15">
+      <c r="A14" s="15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" customFormat="1" s="15">
+      <c r="A15" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" s="15">
+      <c r="A16" s="15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" s="15">
+      <c r="A17" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" s="15">
+      <c r="A18" s="15" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" s="15">
+      <c r="A19" s="15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" customFormat="1" s="15">
+      <c r="A20" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" customFormat="1" s="15">
+      <c r="A21" s="15" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="22" customFormat="1" s="15">
+      <c r="A22" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="23" customFormat="1" s="15">
+      <c r="A23" s="15" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" customFormat="1" s="15">
+      <c r="A24" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" customFormat="1" s="15">
+      <c r="A25" s="15" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="26" customFormat="1" s="15">
+      <c r="A26" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="27" customFormat="1" s="15">
+      <c r="A27" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" customFormat="1" s="15">
+      <c r="A28" s="26"/>
+    </row>
+    <row r="29" customFormat="1" s="15">
+      <c r="A29" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="30" customFormat="1" s="15">
+      <c r="A30" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" customFormat="1" s="15">
+      <c r="A31" s="15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="32" customFormat="1" s="15">
+      <c r="A32" s="15" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" customFormat="1" s="15">
+      <c r="A33" s="15" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="34" customFormat="1" s="15">
+      <c r="A34" s="15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" customFormat="1" s="15">
+      <c r="A35" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="36" customFormat="1" s="15"/>
+    <row r="37" customFormat="1" s="15">
+      <c r="A37" s="26"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>